<commit_message>
update usecase, bang tien do
</commit_message>
<xml_diff>
--- a/BangBaoCaoTienDoCongViec.xlsx
+++ b/BangBaoCaoTienDoCongViec.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Kết quản thực hiện</t>
   </si>
@@ -80,6 +80,12 @@
     <t xml:space="preserve"> Khảo sát hiện trạng. 
 Vẽ Usecase
 Tìm hiểu công nghệ sử dụng</t>
+  </si>
+  <si>
+    <t>Vẽ Sequence Diagram, Class Diagram, Data flow Diagram(bỏ qua nếu dùng EF(code-first))</t>
+  </si>
+  <si>
+    <t>Edit lại usecase Đăng nhập và thống kê</t>
   </si>
 </sst>
 </file>
@@ -127,10 +133,10 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -415,17 +421,17 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:C16"/>
+      <selection activeCell="C5" sqref="C5:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="27.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="27.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
@@ -433,115 +439,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B7:B8"/>
@@ -549,6 +555,11 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cap nhat them sequence va cap nhat ban tien do cong viec
</commit_message>
<xml_diff>
--- a/BangBaoCaoTienDoCongViec.xlsx
+++ b/BangBaoCaoTienDoCongViec.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10\Desktop\Tiểu Luận\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="6930" windowHeight="7245"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Kết quản thực hiện</t>
   </si>
@@ -77,13 +77,21 @@
     <t>Tuần 15</t>
   </si>
   <si>
-    <t>Sequence Diagram, Class Diagram, Prototype</t>
+    <t xml:space="preserve"> Khảo sát hiện trạng. 
+Vẽ Usecase
+Tìm hiểu công nghệ sử dụng</t>
+  </si>
+  <si>
+    <t>Edit lại usecase Đăng nhập và thống kê</t>
   </si>
   <si>
     <t>Hoàn thành</t>
   </si>
   <si>
-    <t xml:space="preserve"> Khảo sát hiện trạng, Vẽ Usecase,Tìm hiểu công nghệ sử dụng</t>
+    <t>Thiết kế các giao diện cho website</t>
+  </si>
+  <si>
+    <t>Vẽ Sequence Diagram, Class Diagram, Database Diagram, Prototype</t>
   </si>
 </sst>
 </file>
@@ -128,13 +136,13 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -422,127 +430,129 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B5" sqref="B5:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="75.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="82.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>

</xml_diff>